<commit_message>
one workshop for layout + layout name
</commit_message>
<xml_diff>
--- a/omzit_terminal/LayoutPlasmaTemplate.xlsx
+++ b/omzit_terminal/LayoutPlasmaTemplate.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t xml:space="preserve">СЗ</t>
   </si>
@@ -50,6 +50,9 @@
   </si>
   <si>
     <t xml:space="preserve">Материал</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Имя детали на раскладке</t>
   </si>
 </sst>
 </file>
@@ -138,11 +141,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -269,10 +272,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K1" activeCellId="0" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="17.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -285,8 +288,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="23.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="34.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="9.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="72.93"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="11" style="1" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="1" width="72.93"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="12" style="1" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -319,6 +322,9 @@
       </c>
       <c r="J1" s="1" t="s">
         <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>